<commit_message>
Actualizacion lectura cuadro amarillo
</commit_message>
<xml_diff>
--- a/Automatizacion_Banrural/Data/Input/TadminData.xlsx
+++ b/Automatizacion_Banrural/Data/Input/TadminData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Propa34653\Desktop\EY\Banrural\Automatizacion_Banrural\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C4177-44AF-4FB9-92D4-A8BD6A892B57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A72E42-2F99-4AC7-8E4F-70D268BFB239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{70F223A5-183F-4C5B-8746-33CD95BBB22C}"/>
+    <workbookView xWindow="7125" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{D256D0C8-60FC-4857-9930-B777B38766DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>BANCO DE DESARROLLO RURAL, S. A.</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>20:22:31</t>
-  </si>
-  <si>
-    <t>Corr-N/DEBITO PAGO DEORSA BANCA VIRTUAL</t>
   </si>
 </sst>
 </file>
@@ -494,12 +491,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436C02E1-792A-43D2-AACA-4B93BCDDEAA0}">
-  <dimension ref="A1:L15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB976110-C4B7-4D54-9CF7-B6CD60A6924A}">
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,44 +710,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5">
-        <v>583</v>
-      </c>
-      <c r="C15" s="5">
-        <v>948</v>
-      </c>
-      <c r="D15" s="5">
-        <v>503188081</v>
-      </c>
-      <c r="E15" s="5">
-        <v>503188080</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="6">
-        <v>65</v>
-      </c>
-      <c r="I15" s="6">
-        <v>8492.18</v>
-      </c>
-      <c r="J15" s="6">
-        <v>8492.18</v>
-      </c>
-      <c r="K15" s="5">
-        <v>503188080</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>